<commit_message>
Added background color for cells that are changed
</commit_message>
<xml_diff>
--- a/compared.xlsx
+++ b/compared.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="removed" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="added" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="changed" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="removed col" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="added col" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="removed row" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="added row" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="changed row" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="removed col" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="added col" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -33,12 +33,17 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA500"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -60,11 +65,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1506,7 +1512,7 @@
         <v>4</v>
       </c>
       <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="inlineStr">
+      <c r="AN2" s="2" t="inlineStr">
         <is>
           <t>1 ---&gt; 2</t>
         </is>
@@ -1607,7 +1613,7 @@
       <c r="AD3" t="n">
         <v>10000</v>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AE3" s="2" t="inlineStr">
         <is>
           <t>nan ---&gt; Bob</t>
         </is>
@@ -1622,7 +1628,7 @@
         <v>4</v>
       </c>
       <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr">
+      <c r="AN3" s="2" t="inlineStr">
         <is>
           <t>1 ---&gt; 2</t>
         </is>
@@ -1734,7 +1740,7 @@
         <v>4</v>
       </c>
       <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr">
+      <c r="AN4" s="2" t="inlineStr">
         <is>
           <t>1 ---&gt; 2</t>
         </is>
@@ -1766,7 +1772,7 @@
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>nan ---&gt; HQ</t>
         </is>

</xml_diff>